<commit_message>
Sửa lỗi kAI của table taikhoan
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\MVC_QT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B7CEA-5D5A-4138-9526-F0CF7BCD7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348D9F9A-5583-428A-9F64-43091B4BF4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E16C9753-E845-4C4E-827F-AA1A4423BD17}"/>
   </bookViews>
@@ -102,10 +102,10 @@
     <t>TEST USER: cart/voucher/checkout/history/detail history/contact/notification/review/</t>
   </si>
   <si>
-    <t>TEST USER: login/logout/change/forget/register/update info/home/search/filter/product/detail product/comment/</t>
-  </si>
-  <si>
     <t>ADMIN: toàn bộ</t>
+  </si>
+  <si>
+    <t>TEST USER: login/logout/change/register/update info/home/search/product/detail product/comment/</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F3" sqref="F3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +639,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -663,7 +663,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>

</xml_diff>